<commit_message>
More Work On SF2
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf2.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CBNHS System\Project Files\Forms System Final\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A42DA9-420B-4888-BA05-2E6159745E34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2619E196-DD26-463C-ABA4-D71E1B455E2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="15150" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" activeTab="0"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3550" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3724" uniqueCount="108">
   <si>
     <t>M</t>
   </si>
@@ -303,6 +303,93 @@
   </si>
   <si>
     <t xml:space="preserve">FUMINO ONA FURAHASHI </t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Paderogao, Phil Rey, E. Jr</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>T/I: 2020-02-01</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rizal, Jose </t>
+  </si>
+  <si>
+    <t>&lt;==Male Total Per Day==&gt;</t>
+  </si>
+  <si>
+    <t>&lt;==Female Total Per Day==&gt;</t>
+  </si>
+  <si>
+    <t>&lt;==Combined Total Per Day==&gt;</t>
   </si>
 </sst>
 </file>
@@ -457,7 +544,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -627,19 +714,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="thin">
         <color indexed="64"/>
@@ -1158,6 +1232,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1180,7 +1280,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="150">
+  <cellXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
@@ -1256,19 +1356,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" xfId="1" applyBorder="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1278,345 +1375,397 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="2" applyFont="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="2" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="1" applyFont="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="5" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="61" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" xfId="6" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="56" xfId="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="2" applyFont="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="2" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1643,7 +1792,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1671,7 +1820,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1714,6 +1863,44 @@
             </a14:hiddenLine>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Picture"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="true"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="304800" cy="190500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1997,198 +2184,198 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="23.25">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="137" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="43"/>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
-      <c r="Q1" s="43"/>
-      <c r="R1" s="43"/>
-      <c r="S1" s="43"/>
-      <c r="T1" s="43"/>
-      <c r="U1" s="43"/>
-      <c r="V1" s="43"/>
-      <c r="W1" s="43"/>
-      <c r="X1" s="43"/>
-      <c r="Y1" s="43"/>
-      <c r="Z1" s="43"/>
-      <c r="AA1" s="43"/>
-      <c r="AB1" s="43"/>
-      <c r="AC1" s="43"/>
-      <c r="AD1" s="43"/>
+      <c r="B1" s="137"/>
+      <c r="C1" s="137"/>
+      <c r="D1" s="137"/>
+      <c r="E1" s="137"/>
+      <c r="F1" s="137"/>
+      <c r="G1" s="137"/>
+      <c r="H1" s="137"/>
+      <c r="I1" s="137"/>
+      <c r="J1" s="137"/>
+      <c r="K1" s="137"/>
+      <c r="L1" s="137"/>
+      <c r="M1" s="137"/>
+      <c r="N1" s="137"/>
+      <c r="O1" s="137"/>
+      <c r="P1" s="137"/>
+      <c r="Q1" s="137"/>
+      <c r="R1" s="137"/>
+      <c r="S1" s="137"/>
+      <c r="T1" s="137"/>
+      <c r="U1" s="137"/>
+      <c r="V1" s="137"/>
+      <c r="W1" s="137"/>
+      <c r="X1" s="137"/>
+      <c r="Y1" s="137"/>
+      <c r="Z1" s="137"/>
+      <c r="AA1" s="137"/>
+      <c r="AB1" s="137"/>
+      <c r="AC1" s="137"/>
+      <c r="AD1" s="137"/>
     </row>
     <row r="2" spans="1:30" ht="9.75" customHeight="1">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="44"/>
-      <c r="R2" s="44"/>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
-      <c r="W2" s="44"/>
-      <c r="X2" s="44"/>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="44"/>
-      <c r="AB2" s="44"/>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="138"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="138"/>
+      <c r="H2" s="138"/>
+      <c r="I2" s="138"/>
+      <c r="J2" s="138"/>
+      <c r="K2" s="138"/>
+      <c r="L2" s="138"/>
+      <c r="M2" s="138"/>
+      <c r="N2" s="138"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="138"/>
+      <c r="Q2" s="138"/>
+      <c r="R2" s="138"/>
+      <c r="S2" s="138"/>
+      <c r="T2" s="138"/>
+      <c r="U2" s="138"/>
+      <c r="V2" s="138"/>
+      <c r="W2" s="138"/>
+      <c r="X2" s="138"/>
+      <c r="Y2" s="138"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="138"/>
+      <c r="AC2" s="138"/>
+      <c r="AD2" s="138"/>
     </row>
     <row r="3" spans="1:30" ht="15.75">
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="36" t="s">
+      <c r="C3" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="148" t="s">
+      <c r="D3" s="139"/>
+      <c r="E3" s="139"/>
+      <c r="F3" s="143" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="148"/>
-      <c r="H3" s="149"/>
-      <c r="I3" s="45" t="s">
+      <c r="G3" s="143"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="140" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="46"/>
-      <c r="K3" s="46"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="40" t="s">
+      <c r="J3" s="141"/>
+      <c r="K3" s="141"/>
+      <c r="L3" s="142"/>
+      <c r="M3" s="148" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="41"/>
-      <c r="O3" s="41"/>
-      <c r="P3" s="41"/>
-      <c r="Q3" s="42"/>
-      <c r="R3" s="36" t="s">
+      <c r="N3" s="149"/>
+      <c r="O3" s="149"/>
+      <c r="P3" s="149"/>
+      <c r="Q3" s="150"/>
+      <c r="R3" s="139" t="s">
         <v>72</v>
       </c>
-      <c r="S3" s="36"/>
-      <c r="T3" s="36"/>
-      <c r="U3" s="36"/>
-      <c r="V3" s="36"/>
-      <c r="W3" s="36"/>
-      <c r="X3" s="36"/>
+      <c r="S3" s="139"/>
+      <c r="T3" s="139"/>
+      <c r="U3" s="139"/>
+      <c r="V3" s="139"/>
+      <c r="W3" s="139"/>
+      <c r="X3" s="139"/>
     </row>
     <row r="4" spans="1:30" ht="16.5" thickBot="1">
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="37" t="s">
+      <c r="D4" s="139"/>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="139"/>
+      <c r="L4" s="139"/>
+      <c r="M4" s="145" t="s">
         <v>16</v>
       </c>
-      <c r="N4" s="38"/>
-      <c r="O4" s="38"/>
-      <c r="P4" s="38"/>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="36" t="s">
+      <c r="N4" s="146"/>
+      <c r="O4" s="146"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="147"/>
+      <c r="R4" s="139" t="s">
         <v>75</v>
       </c>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="37" t="s">
+      <c r="S4" s="139"/>
+      <c r="T4" s="139"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="139"/>
+      <c r="W4" s="139"/>
+      <c r="X4" s="139"/>
+      <c r="Y4" s="145" t="s">
         <v>17</v>
       </c>
-      <c r="Z4" s="38"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="36" t="s">
+      <c r="Z4" s="146"/>
+      <c r="AA4" s="147"/>
+      <c r="AB4" s="139" t="s">
         <v>76</v>
       </c>
-      <c r="AC4" s="36"/>
-      <c r="AD4" s="36"/>
+      <c r="AC4" s="139"/>
+      <c r="AD4" s="139"/>
     </row>
     <row r="5" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="121" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="49" t="s">
+      <c r="B5" s="122" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="D5" s="50"/>
-      <c r="E5" s="50"/>
-      <c r="F5" s="50"/>
-      <c r="G5" s="50"/>
-      <c r="H5" s="50"/>
-      <c r="I5" s="50"/>
-      <c r="J5" s="50"/>
-      <c r="K5" s="50"/>
-      <c r="L5" s="50"/>
-      <c r="M5" s="50"/>
-      <c r="N5" s="50"/>
-      <c r="O5" s="50"/>
-      <c r="P5" s="50"/>
-      <c r="Q5" s="50"/>
-      <c r="R5" s="50"/>
-      <c r="S5" s="50"/>
-      <c r="T5" s="50"/>
-      <c r="U5" s="50"/>
-      <c r="V5" s="50"/>
-      <c r="W5" s="50"/>
-      <c r="X5" s="50"/>
-      <c r="Y5" s="50"/>
-      <c r="Z5" s="50"/>
-      <c r="AA5" s="50"/>
-      <c r="AB5" s="35" t="s">
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
+      <c r="H5" s="123"/>
+      <c r="I5" s="123"/>
+      <c r="J5" s="123"/>
+      <c r="K5" s="123"/>
+      <c r="L5" s="123"/>
+      <c r="M5" s="123"/>
+      <c r="N5" s="123"/>
+      <c r="O5" s="123"/>
+      <c r="P5" s="123"/>
+      <c r="Q5" s="123"/>
+      <c r="R5" s="123"/>
+      <c r="S5" s="123"/>
+      <c r="T5" s="123"/>
+      <c r="U5" s="123"/>
+      <c r="V5" s="123"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="123"/>
+      <c r="Y5" s="123"/>
+      <c r="Z5" s="123"/>
+      <c r="AA5" s="123"/>
+      <c r="AB5" s="124" t="s">
         <v>7</v>
       </c>
-      <c r="AC5" s="35"/>
-      <c r="AD5" s="35" t="s">
+      <c r="AC5" s="124"/>
+      <c r="AD5" s="124" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A6" s="48"/>
-      <c r="B6" s="48"/>
+      <c r="A6" s="121"/>
+      <c r="B6" s="121"/>
       <c r="C6" s="1" t="s">
         <v>20</v>
       </c>
@@ -2204,33 +2391,73 @@
       <c r="G6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="4"/>
-      <c r="R6" s="1"/>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1"/>
-      <c r="U6" s="1"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="1"/>
-      <c r="X6" s="1"/>
-      <c r="Y6" s="1"/>
-      <c r="Z6" s="1"/>
-      <c r="AA6" s="4"/>
-      <c r="AB6" s="35"/>
-      <c r="AC6" s="35"/>
-      <c r="AD6" s="35"/>
+      <c r="H6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="U6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AA6" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="AB6" s="124"/>
+      <c r="AC6" s="124"/>
+      <c r="AD6" s="124"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" thickBot="1">
-      <c r="A7" s="48"/>
-      <c r="B7" s="48"/>
+      <c r="A7" s="121"/>
+      <c r="B7" s="121"/>
       <c r="C7" s="6" t="s">
         <v>0</v>
       </c>
@@ -2312,78 +2539,198 @@
       <c r="AC7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="AD7" s="35"/>
+      <c r="AD7" s="124"/>
     </row>
     <row r="8" spans="1:30">
-      <c r="A8" s="3"/>
-      <c r="B8" s="9"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="11"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-      <c r="Y8" s="1"/>
-      <c r="Z8" s="1"/>
-      <c r="AA8" s="1"/>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
+      <c r="A8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="AD8" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:30">
-      <c r="A9" s="3"/>
-      <c r="B9" s="9"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="4"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
+      <c r="A9" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="P9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AC9" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD9" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>20</v>
+        <v>105</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -2416,22 +2763,22 @@
         <v>20</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="N10" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="O10" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="Q10" s="4" t="s">
         <v>20</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="S10" s="1" t="s">
         <v>20</v>
@@ -2461,10 +2808,10 @@
         <v>20</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="AD10" s="3"/>
     </row>
@@ -2473,7 +2820,7 @@
         <v>20</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>20</v>
+        <v>106</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
@@ -2506,22 +2853,22 @@
         <v>20</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="4" t="s">
         <v>20</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="S11" s="1" t="s">
         <v>20</v>
@@ -2551,10 +2898,10 @@
         <v>20</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="AD11" s="3"/>
     </row>
@@ -2563,7 +2910,7 @@
         <v>20</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>20</v>
+        <v>107</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>20</v>
@@ -2596,22 +2943,22 @@
         <v>20</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="Q12" s="4" t="s">
         <v>20</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="S12" s="1" t="s">
         <v>20</v>
@@ -2641,10 +2988,10 @@
         <v>20</v>
       </c>
       <c r="AB12" s="3" t="s">
-        <v>20</v>
+        <v>103</v>
       </c>
       <c r="AC12" s="3" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="AD12" s="3"/>
     </row>
@@ -3221,42 +3568,42 @@
       <c r="AD19" s="3"/>
     </row>
     <row r="20" spans="1:38" ht="15.75" thickBot="1">
-      <c r="A20" s="3"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="1"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="1"/>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="1"/>
-      <c r="Y20" s="1"/>
-      <c r="Z20" s="1"/>
-      <c r="AA20" s="1"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="3"/>
-      <c r="AD20" s="3"/>
+      <c r="A20" s="158"/>
+      <c r="B20" s="159"/>
+      <c r="C20" s="160"/>
+      <c r="D20" s="160"/>
+      <c r="E20" s="160"/>
+      <c r="F20" s="160"/>
+      <c r="G20" s="161"/>
+      <c r="H20" s="160"/>
+      <c r="I20" s="160"/>
+      <c r="J20" s="160"/>
+      <c r="K20" s="160"/>
+      <c r="L20" s="161"/>
+      <c r="M20" s="160"/>
+      <c r="N20" s="160"/>
+      <c r="O20" s="160"/>
+      <c r="P20" s="160"/>
+      <c r="Q20" s="161"/>
+      <c r="R20" s="160"/>
+      <c r="S20" s="160"/>
+      <c r="T20" s="160"/>
+      <c r="U20" s="160"/>
+      <c r="V20" s="161"/>
+      <c r="W20" s="160"/>
+      <c r="X20" s="160"/>
+      <c r="Y20" s="160"/>
+      <c r="Z20" s="160"/>
+      <c r="AA20" s="160"/>
+      <c r="AB20" s="158"/>
+      <c r="AC20" s="158"/>
+      <c r="AD20" s="158"/>
     </row>
     <row r="21" spans="1:38" ht="17.25" customHeight="1">
-      <c r="A21" s="124" t="s">
+      <c r="A21" s="151" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="124"/>
+      <c r="B21" s="151"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="14"/>
@@ -3265,143 +3612,143 @@
       <c r="H21" s="14"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
-      <c r="K21" s="96" t="s">
+      <c r="K21" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="L21" s="97"/>
-      <c r="M21" s="97"/>
-      <c r="N21" s="97"/>
-      <c r="O21" s="97"/>
-      <c r="P21" s="97"/>
-      <c r="Q21" s="97"/>
-      <c r="R21" s="97"/>
-      <c r="S21" s="28"/>
-      <c r="T21" s="57" t="s">
+      <c r="L21" s="42"/>
+      <c r="M21" s="42"/>
+      <c r="N21" s="42"/>
+      <c r="O21" s="42"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="42"/>
+      <c r="R21" s="42"/>
+      <c r="S21" s="29"/>
+      <c r="T21" s="152" t="s">
         <v>24</v>
       </c>
-      <c r="U21" s="58"/>
-      <c r="V21" s="59"/>
-      <c r="W21" s="63" t="s">
+      <c r="U21" s="153"/>
+      <c r="V21" s="154"/>
+      <c r="W21" s="155" t="s">
         <v>25</v>
       </c>
-      <c r="X21" s="64"/>
+      <c r="X21" s="156"/>
       <c r="Y21" s="74" t="s">
         <v>26</v>
       </c>
       <c r="Z21" s="75"/>
       <c r="AA21" s="75"/>
-      <c r="AB21" s="76"/>
+      <c r="AB21" s="157"/>
       <c r="AL21" s="12"/>
     </row>
     <row r="22" spans="1:38" ht="15" customHeight="1" thickBot="1">
-      <c r="A22" s="122" t="s">
+      <c r="A22" s="65" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="122"/>
-      <c r="C22" s="122"/>
-      <c r="D22" s="122"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
       <c r="H22" s="14"/>
       <c r="I22" s="14"/>
       <c r="J22" s="14"/>
-      <c r="K22" s="98" t="s">
+      <c r="K22" s="135" t="s">
         <v>28</v>
       </c>
-      <c r="L22" s="99"/>
-      <c r="M22" s="99"/>
-      <c r="N22" s="99"/>
-      <c r="O22" s="99"/>
-      <c r="P22" s="99"/>
-      <c r="Q22" s="99"/>
-      <c r="R22" s="99"/>
-      <c r="S22" s="29"/>
-      <c r="T22" s="60" t="s">
+      <c r="L22" s="136"/>
+      <c r="M22" s="136"/>
+      <c r="N22" s="136"/>
+      <c r="O22" s="136"/>
+      <c r="P22" s="136"/>
+      <c r="Q22" s="136"/>
+      <c r="R22" s="136"/>
+      <c r="S22" s="28"/>
+      <c r="T22" s="128" t="s">
         <v>72</v>
       </c>
-      <c r="U22" s="61"/>
-      <c r="V22" s="62"/>
-      <c r="W22" s="60" t="s">
+      <c r="U22" s="129"/>
+      <c r="V22" s="130"/>
+      <c r="W22" s="128" t="s">
         <v>77</v>
       </c>
-      <c r="X22" s="62"/>
+      <c r="X22" s="130"/>
       <c r="Y22" s="13" t="s">
         <v>0</v>
       </c>
       <c r="Z22" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="AA22" s="77" t="s">
+      <c r="AA22" s="111" t="s">
         <v>29</v>
       </c>
-      <c r="AB22" s="78"/>
+      <c r="AB22" s="112"/>
       <c r="AL22" s="12"/>
     </row>
     <row r="23" spans="1:38">
-      <c r="A23" s="122"/>
-      <c r="B23" s="122"/>
-      <c r="C23" s="122"/>
-      <c r="D23" s="122"/>
+      <c r="A23" s="65"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="65"/>
+      <c r="D23" s="65"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
       <c r="I23" s="14"/>
       <c r="J23" s="14"/>
-      <c r="K23" s="98"/>
-      <c r="L23" s="99"/>
-      <c r="M23" s="99"/>
-      <c r="N23" s="99"/>
-      <c r="O23" s="99"/>
-      <c r="P23" s="99"/>
-      <c r="Q23" s="99"/>
-      <c r="R23" s="99"/>
-      <c r="S23" s="29"/>
-      <c r="T23" s="79" t="s">
+      <c r="K23" s="135"/>
+      <c r="L23" s="136"/>
+      <c r="M23" s="136"/>
+      <c r="N23" s="136"/>
+      <c r="O23" s="136"/>
+      <c r="P23" s="136"/>
+      <c r="Q23" s="136"/>
+      <c r="R23" s="136"/>
+      <c r="S23" s="28"/>
+      <c r="T23" s="113" t="s">
         <v>30</v>
       </c>
-      <c r="U23" s="80"/>
-      <c r="V23" s="80"/>
-      <c r="W23" s="80"/>
-      <c r="X23" s="81"/>
-      <c r="Y23" s="85"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="53"/>
-      <c r="AB23" s="54"/>
+      <c r="U23" s="114"/>
+      <c r="V23" s="114"/>
+      <c r="W23" s="114"/>
+      <c r="X23" s="115"/>
+      <c r="Y23" s="119"/>
+      <c r="Z23" s="99"/>
+      <c r="AA23" s="102"/>
+      <c r="AB23" s="103"/>
       <c r="AL23" s="12"/>
     </row>
     <row r="24" spans="1:38" ht="14.45" customHeight="1">
-      <c r="A24" s="122"/>
-      <c r="B24" s="122"/>
-      <c r="C24" s="122"/>
-      <c r="D24" s="122"/>
+      <c r="A24" s="65"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="65"/>
+      <c r="D24" s="65"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
       <c r="H24" s="14"/>
       <c r="I24" s="14"/>
       <c r="J24" s="14"/>
-      <c r="K24" s="100" t="s">
+      <c r="K24" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="L24" s="101"/>
-      <c r="M24" s="101"/>
-      <c r="N24" s="101"/>
-      <c r="O24" s="101"/>
-      <c r="P24" s="101"/>
-      <c r="Q24" s="101"/>
-      <c r="R24" s="101"/>
-      <c r="S24" s="30"/>
-      <c r="T24" s="82"/>
-      <c r="U24" s="83"/>
-      <c r="V24" s="83"/>
-      <c r="W24" s="83"/>
-      <c r="X24" s="84"/>
-      <c r="Y24" s="86"/>
-      <c r="Z24" s="52"/>
-      <c r="AA24" s="55"/>
-      <c r="AB24" s="56"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="42"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="42"/>
+      <c r="R24" s="42"/>
+      <c r="S24" s="29"/>
+      <c r="T24" s="116"/>
+      <c r="U24" s="117"/>
+      <c r="V24" s="117"/>
+      <c r="W24" s="117"/>
+      <c r="X24" s="118"/>
+      <c r="Y24" s="120"/>
+      <c r="Z24" s="101"/>
+      <c r="AA24" s="106"/>
+      <c r="AB24" s="107"/>
       <c r="AL24" s="12"/>
     </row>
     <row r="25" spans="1:38" ht="14.45" customHeight="1">
@@ -3415,17 +3762,17 @@
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
       <c r="J25" s="14"/>
-      <c r="K25" s="100" t="s">
+      <c r="K25" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="L25" s="101"/>
-      <c r="M25" s="101"/>
-      <c r="N25" s="101"/>
-      <c r="O25" s="101"/>
-      <c r="P25" s="101"/>
-      <c r="Q25" s="101"/>
-      <c r="R25" s="101"/>
-      <c r="S25" s="30"/>
+      <c r="L25" s="42"/>
+      <c r="M25" s="42"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="42"/>
+      <c r="R25" s="42"/>
+      <c r="S25" s="29"/>
       <c r="T25" s="89" t="s">
         <v>32</v>
       </c>
@@ -3435,15 +3782,15 @@
         <v>33</v>
       </c>
       <c r="X25" s="93"/>
-      <c r="Y25" s="51"/>
-      <c r="Z25" s="51"/>
-      <c r="AA25" s="53"/>
-      <c r="AB25" s="54"/>
+      <c r="Y25" s="99"/>
+      <c r="Z25" s="99"/>
+      <c r="AA25" s="102"/>
+      <c r="AB25" s="103"/>
       <c r="AL25" s="12"/>
     </row>
     <row r="26" spans="1:38" ht="14.45" customHeight="1">
       <c r="A26" s="12"/>
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="36" t="s">
         <v>34</v>
       </c>
       <c r="C26" s="88" t="s">
@@ -3454,70 +3801,70 @@
       <c r="F26" s="88"/>
       <c r="G26" s="88"/>
       <c r="H26" s="88"/>
-      <c r="I26" s="87" t="s">
+      <c r="I26" s="36" t="s">
         <v>36</v>
       </c>
       <c r="J26" s="15"/>
-      <c r="K26" s="137" t="s">
+      <c r="K26" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="L26" s="135"/>
-      <c r="M26" s="135"/>
-      <c r="N26" s="135"/>
-      <c r="O26" s="135"/>
-      <c r="P26" s="135"/>
-      <c r="Q26" s="135"/>
-      <c r="R26" s="138"/>
-      <c r="S26" s="30"/>
+      <c r="L26" s="39"/>
+      <c r="M26" s="39"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="39"/>
+      <c r="P26" s="39"/>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="40"/>
+      <c r="S26" s="29"/>
       <c r="T26" s="89"/>
       <c r="U26" s="90"/>
       <c r="V26" s="91"/>
       <c r="W26" s="92"/>
       <c r="X26" s="93"/>
-      <c r="Y26" s="65"/>
-      <c r="Z26" s="65"/>
-      <c r="AA26" s="66"/>
-      <c r="AB26" s="67"/>
+      <c r="Y26" s="100"/>
+      <c r="Z26" s="100"/>
+      <c r="AA26" s="104"/>
+      <c r="AB26" s="105"/>
       <c r="AL26" s="12"/>
     </row>
     <row r="27" spans="1:38" ht="12.6" customHeight="1">
       <c r="A27" s="12"/>
-      <c r="B27" s="87"/>
-      <c r="C27" s="136" t="s">
+      <c r="B27" s="36"/>
+      <c r="C27" s="98" t="s">
         <v>39</v>
       </c>
-      <c r="D27" s="136"/>
-      <c r="E27" s="136"/>
-      <c r="F27" s="136"/>
-      <c r="G27" s="136"/>
-      <c r="H27" s="136"/>
-      <c r="I27" s="95"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="98"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="98"/>
+      <c r="H27" s="98"/>
+      <c r="I27" s="37"/>
       <c r="J27" s="16"/>
-      <c r="K27" s="137"/>
-      <c r="L27" s="135"/>
-      <c r="M27" s="135"/>
-      <c r="N27" s="135"/>
-      <c r="O27" s="135"/>
-      <c r="P27" s="135"/>
-      <c r="Q27" s="135"/>
-      <c r="R27" s="138"/>
-      <c r="S27" s="30"/>
-      <c r="T27" s="68" t="s">
+      <c r="K27" s="38"/>
+      <c r="L27" s="39"/>
+      <c r="M27" s="39"/>
+      <c r="N27" s="39"/>
+      <c r="O27" s="39"/>
+      <c r="P27" s="39"/>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="40"/>
+      <c r="S27" s="29"/>
+      <c r="T27" s="95" t="s">
         <v>38</v>
       </c>
-      <c r="U27" s="69"/>
-      <c r="V27" s="69"/>
-      <c r="W27" s="69"/>
-      <c r="X27" s="70"/>
-      <c r="Y27" s="65"/>
-      <c r="Z27" s="65"/>
-      <c r="AA27" s="66"/>
-      <c r="AB27" s="67"/>
+      <c r="U27" s="96"/>
+      <c r="V27" s="96"/>
+      <c r="W27" s="96"/>
+      <c r="X27" s="97"/>
+      <c r="Y27" s="100"/>
+      <c r="Z27" s="100"/>
+      <c r="AA27" s="104"/>
+      <c r="AB27" s="105"/>
       <c r="AL27" s="12"/>
     </row>
     <row r="28" spans="1:38" ht="14.45" customHeight="1">
       <c r="A28" s="12"/>
-      <c r="B28" s="87" t="s">
+      <c r="B28" s="36" t="s">
         <v>41</v>
       </c>
       <c r="C28" s="88" t="s">
@@ -3530,67 +3877,67 @@
       <c r="H28" s="88"/>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
-      <c r="K28" s="137"/>
-      <c r="L28" s="135"/>
-      <c r="M28" s="135"/>
-      <c r="N28" s="135"/>
-      <c r="O28" s="135"/>
-      <c r="P28" s="135"/>
-      <c r="Q28" s="135"/>
-      <c r="R28" s="138"/>
-      <c r="S28" s="29"/>
-      <c r="T28" s="71"/>
-      <c r="U28" s="72"/>
-      <c r="V28" s="72"/>
-      <c r="W28" s="72"/>
-      <c r="X28" s="73"/>
-      <c r="Y28" s="52"/>
-      <c r="Z28" s="52"/>
-      <c r="AA28" s="55"/>
-      <c r="AB28" s="56"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="39"/>
+      <c r="M28" s="39"/>
+      <c r="N28" s="39"/>
+      <c r="O28" s="39"/>
+      <c r="P28" s="39"/>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="40"/>
+      <c r="S28" s="28"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="60"/>
+      <c r="V28" s="60"/>
+      <c r="W28" s="60"/>
+      <c r="X28" s="61"/>
+      <c r="Y28" s="101"/>
+      <c r="Z28" s="101"/>
+      <c r="AA28" s="106"/>
+      <c r="AB28" s="107"/>
       <c r="AL28" s="12"/>
     </row>
     <row r="29" spans="1:38" ht="14.45" customHeight="1">
       <c r="A29" s="12"/>
-      <c r="B29" s="87"/>
-      <c r="C29" s="136" t="s">
+      <c r="B29" s="36"/>
+      <c r="C29" s="98" t="s">
         <v>44</v>
       </c>
-      <c r="D29" s="136"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="136"/>
-      <c r="G29" s="136"/>
-      <c r="H29" s="136"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="98"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="98"/>
+      <c r="H29" s="98"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
-      <c r="K29" s="100" t="s">
+      <c r="K29" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="L29" s="101"/>
-      <c r="M29" s="101"/>
-      <c r="N29" s="101"/>
-      <c r="O29" s="101"/>
-      <c r="P29" s="101"/>
-      <c r="Q29" s="101"/>
-      <c r="R29" s="101"/>
-      <c r="S29" s="31"/>
-      <c r="T29" s="111" t="s">
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="42"/>
+      <c r="Q29" s="42"/>
+      <c r="R29" s="42"/>
+      <c r="S29" s="30"/>
+      <c r="T29" s="85" t="s">
         <v>43</v>
       </c>
-      <c r="U29" s="112"/>
-      <c r="V29" s="112"/>
-      <c r="W29" s="112"/>
-      <c r="X29" s="113"/>
-      <c r="Y29" s="102" t="s">
+      <c r="U29" s="86"/>
+      <c r="V29" s="86"/>
+      <c r="W29" s="86"/>
+      <c r="X29" s="87"/>
+      <c r="Y29" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="Z29" s="102" t="s">
+      <c r="Z29" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AA29" s="104" t="s">
+      <c r="AA29" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB29" s="105"/>
+      <c r="AB29" s="56"/>
       <c r="AL29" s="12"/>
     </row>
     <row r="30" spans="1:38" ht="14.45" customHeight="1">
@@ -3606,72 +3953,72 @@
       <c r="F30" s="88"/>
       <c r="G30" s="88"/>
       <c r="H30" s="88"/>
-      <c r="I30" s="87" t="s">
+      <c r="I30" s="36" t="s">
         <v>36</v>
       </c>
       <c r="J30" s="16"/>
-      <c r="K30" s="137" t="s">
+      <c r="K30" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="135"/>
-      <c r="M30" s="135"/>
-      <c r="N30" s="135"/>
-      <c r="O30" s="135"/>
-      <c r="P30" s="135"/>
-      <c r="Q30" s="135"/>
-      <c r="R30" s="138"/>
-      <c r="S30" s="31"/>
-      <c r="T30" s="108" t="s">
+      <c r="L30" s="39"/>
+      <c r="M30" s="39"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="39"/>
+      <c r="P30" s="39"/>
+      <c r="Q30" s="39"/>
+      <c r="R30" s="40"/>
+      <c r="S30" s="30"/>
+      <c r="T30" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="U30" s="109"/>
-      <c r="V30" s="109"/>
-      <c r="W30" s="109"/>
-      <c r="X30" s="110"/>
-      <c r="Y30" s="103"/>
-      <c r="Z30" s="103"/>
-      <c r="AA30" s="106"/>
-      <c r="AB30" s="107"/>
+      <c r="U30" s="83"/>
+      <c r="V30" s="83"/>
+      <c r="W30" s="83"/>
+      <c r="X30" s="84"/>
+      <c r="Y30" s="62"/>
+      <c r="Z30" s="62"/>
+      <c r="AA30" s="63"/>
+      <c r="AB30" s="64"/>
       <c r="AL30" s="12"/>
     </row>
     <row r="31" spans="1:38" ht="14.45" customHeight="1">
       <c r="A31" s="12"/>
-      <c r="C31" s="136" t="s">
+      <c r="C31" s="98" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="136"/>
-      <c r="E31" s="136"/>
-      <c r="F31" s="136"/>
-      <c r="G31" s="136"/>
-      <c r="H31" s="136"/>
-      <c r="I31" s="95"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="98"/>
+      <c r="H31" s="98"/>
+      <c r="I31" s="37"/>
       <c r="J31" s="16"/>
-      <c r="K31" s="137"/>
-      <c r="L31" s="135"/>
-      <c r="M31" s="135"/>
-      <c r="N31" s="135"/>
-      <c r="O31" s="135"/>
-      <c r="P31" s="135"/>
-      <c r="Q31" s="135"/>
-      <c r="R31" s="138"/>
-      <c r="S31" s="29"/>
-      <c r="T31" s="111" t="s">
+      <c r="K31" s="38"/>
+      <c r="L31" s="39"/>
+      <c r="M31" s="39"/>
+      <c r="N31" s="39"/>
+      <c r="O31" s="39"/>
+      <c r="P31" s="39"/>
+      <c r="Q31" s="39"/>
+      <c r="R31" s="40"/>
+      <c r="S31" s="28"/>
+      <c r="T31" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="U31" s="112"/>
-      <c r="V31" s="112"/>
-      <c r="W31" s="112"/>
-      <c r="X31" s="113"/>
-      <c r="Y31" s="102" t="s">
+      <c r="U31" s="86"/>
+      <c r="V31" s="86"/>
+      <c r="W31" s="86"/>
+      <c r="X31" s="87"/>
+      <c r="Y31" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="Z31" s="102" t="s">
+      <c r="Z31" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AA31" s="104" t="s">
+      <c r="AA31" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB31" s="105"/>
+      <c r="AB31" s="56"/>
       <c r="AL31" s="12"/>
     </row>
     <row r="32" spans="1:38" ht="14.45" customHeight="1">
@@ -3679,26 +4026,26 @@
       <c r="B32" s="15"/>
       <c r="C32" s="14"/>
       <c r="D32" s="14"/>
-      <c r="K32" s="137"/>
-      <c r="L32" s="135"/>
-      <c r="M32" s="135"/>
-      <c r="N32" s="135"/>
-      <c r="O32" s="135"/>
-      <c r="P32" s="135"/>
-      <c r="Q32" s="135"/>
-      <c r="R32" s="138"/>
-      <c r="S32" s="30"/>
-      <c r="T32" s="108" t="s">
+      <c r="K32" s="38"/>
+      <c r="L32" s="39"/>
+      <c r="M32" s="39"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="39"/>
+      <c r="P32" s="39"/>
+      <c r="Q32" s="39"/>
+      <c r="R32" s="40"/>
+      <c r="S32" s="29"/>
+      <c r="T32" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="U32" s="109"/>
-      <c r="V32" s="109"/>
-      <c r="W32" s="109"/>
-      <c r="X32" s="110"/>
-      <c r="Y32" s="103"/>
-      <c r="Z32" s="103"/>
-      <c r="AA32" s="106"/>
-      <c r="AB32" s="107"/>
+      <c r="U32" s="83"/>
+      <c r="V32" s="83"/>
+      <c r="W32" s="83"/>
+      <c r="X32" s="84"/>
+      <c r="Y32" s="62"/>
+      <c r="Z32" s="62"/>
+      <c r="AA32" s="63"/>
+      <c r="AB32" s="64"/>
       <c r="AL32" s="12"/>
     </row>
     <row r="33" spans="1:38" ht="14.45" customHeight="1">
@@ -3712,145 +4059,145 @@
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
-      <c r="K33" s="137"/>
-      <c r="L33" s="135"/>
-      <c r="M33" s="135"/>
-      <c r="N33" s="135"/>
-      <c r="O33" s="135"/>
-      <c r="P33" s="135"/>
-      <c r="Q33" s="135"/>
-      <c r="R33" s="138"/>
-      <c r="S33" s="29"/>
-      <c r="T33" s="68" t="s">
+      <c r="K33" s="38"/>
+      <c r="L33" s="39"/>
+      <c r="M33" s="39"/>
+      <c r="N33" s="39"/>
+      <c r="O33" s="39"/>
+      <c r="P33" s="39"/>
+      <c r="Q33" s="39"/>
+      <c r="R33" s="40"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="U33" s="69"/>
-      <c r="V33" s="69"/>
-      <c r="W33" s="69"/>
-      <c r="X33" s="70"/>
-      <c r="Y33" s="102" t="s">
+      <c r="U33" s="96"/>
+      <c r="V33" s="96"/>
+      <c r="W33" s="96"/>
+      <c r="X33" s="97"/>
+      <c r="Y33" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="Z33" s="102" t="s">
+      <c r="Z33" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AA33" s="104" t="s">
+      <c r="AA33" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB33" s="105"/>
+      <c r="AB33" s="56"/>
       <c r="AL33" s="12"/>
     </row>
     <row r="34" spans="1:38" ht="14.45" customHeight="1">
-      <c r="A34" s="125" t="s">
+      <c r="A34" s="68" t="s">
         <v>51</v>
       </c>
-      <c r="B34" s="125"/>
-      <c r="C34" s="125"/>
-      <c r="D34" s="125"/>
-      <c r="E34" s="125"/>
-      <c r="F34" s="125"/>
-      <c r="G34" s="125"/>
-      <c r="H34" s="125"/>
-      <c r="I34" s="125"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
       <c r="J34" s="14"/>
-      <c r="K34" s="100" t="s">
+      <c r="K34" s="41" t="s">
         <v>56</v>
       </c>
-      <c r="L34" s="101"/>
-      <c r="M34" s="101"/>
-      <c r="N34" s="101"/>
-      <c r="O34" s="101"/>
-      <c r="P34" s="101"/>
-      <c r="Q34" s="101"/>
-      <c r="R34" s="101"/>
-      <c r="S34" s="31"/>
-      <c r="T34" s="71"/>
-      <c r="U34" s="72"/>
-      <c r="V34" s="72"/>
-      <c r="W34" s="72"/>
-      <c r="X34" s="73"/>
-      <c r="Y34" s="103"/>
-      <c r="Z34" s="103"/>
-      <c r="AA34" s="106"/>
-      <c r="AB34" s="107"/>
+      <c r="L34" s="42"/>
+      <c r="M34" s="42"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="42"/>
+      <c r="Q34" s="42"/>
+      <c r="R34" s="42"/>
+      <c r="S34" s="30"/>
+      <c r="T34" s="59"/>
+      <c r="U34" s="60"/>
+      <c r="V34" s="60"/>
+      <c r="W34" s="60"/>
+      <c r="X34" s="61"/>
+      <c r="Y34" s="62"/>
+      <c r="Z34" s="62"/>
+      <c r="AA34" s="63"/>
+      <c r="AB34" s="64"/>
       <c r="AL34" s="12"/>
     </row>
     <row r="35" spans="1:38">
-      <c r="A35" s="125"/>
-      <c r="B35" s="125"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="125"/>
-      <c r="E35" s="125"/>
-      <c r="F35" s="125"/>
-      <c r="G35" s="125"/>
-      <c r="H35" s="125"/>
-      <c r="I35" s="125"/>
+      <c r="A35" s="68"/>
+      <c r="B35" s="68"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+      <c r="F35" s="68"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="68"/>
       <c r="J35" s="14"/>
-      <c r="K35" s="134" t="s">
+      <c r="K35" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="L35" s="135"/>
-      <c r="M35" s="135"/>
-      <c r="N35" s="135"/>
-      <c r="O35" s="135"/>
-      <c r="P35" s="135"/>
-      <c r="Q35" s="135"/>
-      <c r="R35" s="135"/>
-      <c r="S35" s="31"/>
-      <c r="T35" s="71" t="s">
+      <c r="L35" s="39"/>
+      <c r="M35" s="39"/>
+      <c r="N35" s="39"/>
+      <c r="O35" s="39"/>
+      <c r="P35" s="39"/>
+      <c r="Q35" s="39"/>
+      <c r="R35" s="39"/>
+      <c r="S35" s="30"/>
+      <c r="T35" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="U35" s="72"/>
-      <c r="V35" s="72"/>
-      <c r="W35" s="72"/>
-      <c r="X35" s="73"/>
-      <c r="Y35" s="34" t="s">
+      <c r="U35" s="60"/>
+      <c r="V35" s="60"/>
+      <c r="W35" s="60"/>
+      <c r="X35" s="61"/>
+      <c r="Y35" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="Z35" s="34" t="s">
+      <c r="Z35" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AA35" s="114" t="s">
+      <c r="AA35" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="AB35" s="115"/>
+      <c r="AB35" s="81"/>
       <c r="AL35" s="12"/>
     </row>
     <row r="36" spans="1:38" ht="11.45" customHeight="1">
-      <c r="A36" s="125"/>
-      <c r="B36" s="125"/>
-      <c r="C36" s="125"/>
-      <c r="D36" s="125"/>
-      <c r="E36" s="125"/>
-      <c r="F36" s="125"/>
-      <c r="G36" s="125"/>
-      <c r="H36" s="125"/>
-      <c r="I36" s="125"/>
+      <c r="A36" s="68"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+      <c r="F36" s="68"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="68"/>
+      <c r="I36" s="68"/>
       <c r="J36" s="14"/>
-      <c r="K36" s="134"/>
-      <c r="L36" s="135"/>
-      <c r="M36" s="135"/>
-      <c r="N36" s="135"/>
-      <c r="O36" s="135"/>
-      <c r="P36" s="135"/>
-      <c r="Q36" s="135"/>
-      <c r="R36" s="135"/>
-      <c r="S36" s="31"/>
-      <c r="T36" s="71" t="s">
+      <c r="K36" s="45"/>
+      <c r="L36" s="39"/>
+      <c r="M36" s="39"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="39"/>
+      <c r="P36" s="39"/>
+      <c r="Q36" s="39"/>
+      <c r="R36" s="39"/>
+      <c r="S36" s="30"/>
+      <c r="T36" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="U36" s="72"/>
-      <c r="V36" s="72"/>
-      <c r="W36" s="72"/>
-      <c r="X36" s="73"/>
-      <c r="Y36" s="34"/>
-      <c r="Z36" s="34" t="s">
+      <c r="U36" s="60"/>
+      <c r="V36" s="60"/>
+      <c r="W36" s="60"/>
+      <c r="X36" s="61"/>
+      <c r="Y36" s="33"/>
+      <c r="Z36" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="AA36" s="114" t="s">
+      <c r="AA36" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="AB36" s="115"/>
+      <c r="AB36" s="81"/>
       <c r="AL36" s="12"/>
     </row>
     <row r="37" spans="1:38" ht="15" customHeight="1">
@@ -3864,41 +4211,41 @@
       <c r="H37" s="14"/>
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
-      <c r="K37" s="100" t="s">
+      <c r="K37" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="L37" s="101"/>
-      <c r="M37" s="101"/>
-      <c r="N37" s="101"/>
-      <c r="O37" s="101"/>
-      <c r="P37" s="101"/>
-      <c r="Q37" s="101"/>
-      <c r="R37" s="101"/>
-      <c r="S37" s="29"/>
-      <c r="T37" s="116" t="s">
+      <c r="L37" s="42"/>
+      <c r="M37" s="42"/>
+      <c r="N37" s="42"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="42"/>
+      <c r="Q37" s="42"/>
+      <c r="R37" s="42"/>
+      <c r="S37" s="28"/>
+      <c r="T37" s="71" t="s">
         <v>54</v>
       </c>
-      <c r="U37" s="117"/>
-      <c r="V37" s="117"/>
-      <c r="W37" s="117"/>
-      <c r="X37" s="118"/>
-      <c r="Y37" s="102" t="s">
+      <c r="U37" s="72"/>
+      <c r="V37" s="72"/>
+      <c r="W37" s="72"/>
+      <c r="X37" s="73"/>
+      <c r="Y37" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="Z37" s="102" t="s">
+      <c r="Z37" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AA37" s="104" t="s">
+      <c r="AA37" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB37" s="105"/>
+      <c r="AB37" s="56"/>
       <c r="AL37" s="12"/>
     </row>
     <row r="38" spans="1:38" ht="14.45" customHeight="1">
       <c r="A38" s="94" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="95"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="17"/>
       <c r="D38" s="17"/>
       <c r="E38" s="17"/>
@@ -3907,26 +4254,26 @@
       <c r="H38" s="17"/>
       <c r="I38" s="17"/>
       <c r="J38" s="17"/>
-      <c r="K38" s="134" t="s">
+      <c r="K38" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="L38" s="135"/>
-      <c r="M38" s="135"/>
-      <c r="N38" s="135"/>
-      <c r="O38" s="135"/>
-      <c r="P38" s="135"/>
-      <c r="Q38" s="135"/>
-      <c r="R38" s="135"/>
-      <c r="S38" s="29"/>
-      <c r="T38" s="119"/>
-      <c r="U38" s="120"/>
-      <c r="V38" s="120"/>
-      <c r="W38" s="120"/>
-      <c r="X38" s="121"/>
-      <c r="Y38" s="103"/>
-      <c r="Z38" s="103"/>
-      <c r="AA38" s="106"/>
-      <c r="AB38" s="107"/>
+      <c r="L38" s="39"/>
+      <c r="M38" s="39"/>
+      <c r="N38" s="39"/>
+      <c r="O38" s="39"/>
+      <c r="P38" s="39"/>
+      <c r="Q38" s="39"/>
+      <c r="R38" s="39"/>
+      <c r="S38" s="28"/>
+      <c r="T38" s="74"/>
+      <c r="U38" s="75"/>
+      <c r="V38" s="75"/>
+      <c r="W38" s="75"/>
+      <c r="X38" s="76"/>
+      <c r="Y38" s="62"/>
+      <c r="Z38" s="62"/>
+      <c r="AA38" s="63"/>
+      <c r="AB38" s="64"/>
       <c r="AL38" s="12"/>
     </row>
     <row r="39" spans="1:38">
@@ -3940,32 +4287,32 @@
       <c r="H39" s="14"/>
       <c r="I39" s="14"/>
       <c r="J39" s="14"/>
-      <c r="K39" s="134"/>
-      <c r="L39" s="135"/>
-      <c r="M39" s="135"/>
-      <c r="N39" s="135"/>
-      <c r="O39" s="135"/>
-      <c r="P39" s="135"/>
-      <c r="Q39" s="135"/>
-      <c r="R39" s="135"/>
-      <c r="S39" s="29"/>
-      <c r="T39" s="116" t="s">
+      <c r="K39" s="45"/>
+      <c r="L39" s="39"/>
+      <c r="M39" s="39"/>
+      <c r="N39" s="39"/>
+      <c r="O39" s="39"/>
+      <c r="P39" s="39"/>
+      <c r="Q39" s="39"/>
+      <c r="R39" s="39"/>
+      <c r="S39" s="28"/>
+      <c r="T39" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="U39" s="117"/>
-      <c r="V39" s="117"/>
-      <c r="W39" s="117"/>
-      <c r="X39" s="118"/>
-      <c r="Y39" s="102" t="s">
+      <c r="U39" s="72"/>
+      <c r="V39" s="72"/>
+      <c r="W39" s="72"/>
+      <c r="X39" s="73"/>
+      <c r="Y39" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="Z39" s="102" t="s">
+      <c r="Z39" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AA39" s="104" t="s">
+      <c r="AA39" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB39" s="105"/>
+      <c r="AB39" s="56"/>
       <c r="AL39" s="12"/>
     </row>
     <row r="40" spans="1:38" ht="14.45" customHeight="1">
@@ -3979,26 +4326,26 @@
       <c r="H40" s="14"/>
       <c r="I40" s="14"/>
       <c r="J40" s="14"/>
-      <c r="K40" s="100" t="s">
+      <c r="K40" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="L40" s="101"/>
-      <c r="M40" s="101"/>
-      <c r="N40" s="101"/>
-      <c r="O40" s="101"/>
-      <c r="P40" s="101"/>
-      <c r="Q40" s="101"/>
-      <c r="R40" s="101"/>
-      <c r="S40" s="29"/>
-      <c r="T40" s="119"/>
-      <c r="U40" s="120"/>
-      <c r="V40" s="120"/>
-      <c r="W40" s="120"/>
-      <c r="X40" s="121"/>
-      <c r="Y40" s="103"/>
-      <c r="Z40" s="103"/>
-      <c r="AA40" s="106"/>
-      <c r="AB40" s="107"/>
+      <c r="L40" s="42"/>
+      <c r="M40" s="42"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="42"/>
+      <c r="Q40" s="42"/>
+      <c r="R40" s="42"/>
+      <c r="S40" s="28"/>
+      <c r="T40" s="74"/>
+      <c r="U40" s="75"/>
+      <c r="V40" s="75"/>
+      <c r="W40" s="75"/>
+      <c r="X40" s="76"/>
+      <c r="Y40" s="62"/>
+      <c r="Z40" s="62"/>
+      <c r="AA40" s="63"/>
+      <c r="AB40" s="64"/>
       <c r="AL40" s="12"/>
     </row>
     <row r="41" spans="1:38" ht="10.9" customHeight="1">
@@ -4012,34 +4359,34 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
       <c r="J41" s="20"/>
-      <c r="K41" s="134" t="s">
+      <c r="K41" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="L41" s="135"/>
-      <c r="M41" s="135"/>
-      <c r="N41" s="135"/>
-      <c r="O41" s="135"/>
-      <c r="P41" s="135"/>
-      <c r="Q41" s="135"/>
-      <c r="R41" s="135"/>
-      <c r="S41" s="31"/>
-      <c r="T41" s="116" t="s">
+      <c r="L41" s="39"/>
+      <c r="M41" s="39"/>
+      <c r="N41" s="39"/>
+      <c r="O41" s="39"/>
+      <c r="P41" s="39"/>
+      <c r="Q41" s="39"/>
+      <c r="R41" s="39"/>
+      <c r="S41" s="30"/>
+      <c r="T41" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="U41" s="117"/>
-      <c r="V41" s="117"/>
-      <c r="W41" s="117"/>
-      <c r="X41" s="118"/>
-      <c r="Y41" s="102" t="s">
+      <c r="U41" s="72"/>
+      <c r="V41" s="72"/>
+      <c r="W41" s="72"/>
+      <c r="X41" s="73"/>
+      <c r="Y41" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="Z41" s="102" t="s">
+      <c r="Z41" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="AA41" s="104" t="s">
+      <c r="AA41" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="AB41" s="105"/>
+      <c r="AB41" s="56"/>
       <c r="AL41" s="12"/>
     </row>
     <row r="42" spans="1:38" ht="21.6" customHeight="1" thickBot="1">
@@ -4053,26 +4400,26 @@
       <c r="H42" s="12"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
-      <c r="K42" s="141" t="s">
+      <c r="K42" s="46" t="s">
         <v>66</v>
       </c>
-      <c r="L42" s="142"/>
-      <c r="M42" s="142"/>
-      <c r="N42" s="142"/>
-      <c r="O42" s="142"/>
-      <c r="P42" s="142"/>
-      <c r="Q42" s="142"/>
-      <c r="R42" s="143"/>
-      <c r="S42" s="31"/>
-      <c r="T42" s="128"/>
-      <c r="U42" s="129"/>
-      <c r="V42" s="129"/>
-      <c r="W42" s="129"/>
-      <c r="X42" s="130"/>
-      <c r="Y42" s="131"/>
-      <c r="Z42" s="131"/>
-      <c r="AA42" s="132"/>
-      <c r="AB42" s="133"/>
+      <c r="L42" s="47"/>
+      <c r="M42" s="47"/>
+      <c r="N42" s="47"/>
+      <c r="O42" s="47"/>
+      <c r="P42" s="47"/>
+      <c r="Q42" s="47"/>
+      <c r="R42" s="48"/>
+      <c r="S42" s="30"/>
+      <c r="T42" s="77"/>
+      <c r="U42" s="78"/>
+      <c r="V42" s="78"/>
+      <c r="W42" s="78"/>
+      <c r="X42" s="79"/>
+      <c r="Y42" s="54"/>
+      <c r="Z42" s="54"/>
+      <c r="AA42" s="57"/>
+      <c r="AB42" s="58"/>
       <c r="AL42" s="12"/>
     </row>
     <row r="43" spans="1:38">
@@ -4117,24 +4464,24 @@
       <c r="H44" s="12"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
-      <c r="K44" s="145"/>
-      <c r="L44" s="145"/>
-      <c r="M44" s="145"/>
-      <c r="N44" s="145"/>
-      <c r="O44" s="145"/>
-      <c r="P44" s="145"/>
-      <c r="Q44" s="145"/>
-      <c r="R44" s="145"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="50"/>
+      <c r="Q44" s="50"/>
+      <c r="R44" s="50"/>
       <c r="S44" s="23"/>
-      <c r="T44" s="146" t="s">
+      <c r="T44" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="U44" s="146"/>
-      <c r="V44" s="146"/>
-      <c r="W44" s="146"/>
-      <c r="X44" s="146"/>
-      <c r="Y44" s="146"/>
-      <c r="Z44" s="146"/>
+      <c r="U44" s="51"/>
+      <c r="V44" s="51"/>
+      <c r="W44" s="51"/>
+      <c r="X44" s="51"/>
+      <c r="Y44" s="51"/>
+      <c r="Z44" s="51"/>
       <c r="AA44" s="14"/>
       <c r="AB44" s="14"/>
       <c r="AL44" s="12"/>
@@ -4150,23 +4497,23 @@
       <c r="H45" s="12"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
-      <c r="M45" s="144" t="s">
+      <c r="M45" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="N45" s="144"/>
-      <c r="O45" s="144"/>
-      <c r="P45" s="144"/>
+      <c r="N45" s="49"/>
+      <c r="O45" s="49"/>
+      <c r="P45" s="49"/>
       <c r="T45" s="14"/>
-      <c r="U45" s="147" t="s">
+      <c r="U45" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="V45" s="147"/>
-      <c r="W45" s="147"/>
-      <c r="X45" s="147"/>
-      <c r="Y45" s="147"/>
-      <c r="Z45" s="147"/>
-      <c r="AA45" s="147"/>
-      <c r="AB45" s="147"/>
+      <c r="V45" s="52"/>
+      <c r="W45" s="52"/>
+      <c r="X45" s="52"/>
+      <c r="Y45" s="52"/>
+      <c r="Z45" s="52"/>
+      <c r="AA45" s="52"/>
+      <c r="AB45" s="52"/>
       <c r="AL45" s="12"/>
     </row>
     <row r="46" spans="1:38" ht="14.45" customHeight="1">
@@ -4181,16 +4528,16 @@
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
       <c r="T46" s="12"/>
-      <c r="U46" s="126" t="s">
+      <c r="U46" s="69" t="s">
         <v>65</v>
       </c>
-      <c r="V46" s="127"/>
-      <c r="W46" s="127"/>
-      <c r="X46" s="127"/>
-      <c r="Y46" s="127"/>
-      <c r="Z46" s="127"/>
-      <c r="AA46" s="127"/>
-      <c r="AB46" s="127"/>
+      <c r="V46" s="70"/>
+      <c r="W46" s="70"/>
+      <c r="X46" s="70"/>
+      <c r="Y46" s="70"/>
+      <c r="Z46" s="70"/>
+      <c r="AA46" s="70"/>
+      <c r="AB46" s="70"/>
       <c r="AL46" s="12"/>
     </row>
     <row r="47" spans="1:38" ht="15" customHeight="1">
@@ -4214,14 +4561,14 @@
       <c r="R47" s="24"/>
       <c r="S47" s="24"/>
       <c r="T47" s="12"/>
-      <c r="U47" s="127"/>
-      <c r="V47" s="127"/>
-      <c r="W47" s="127"/>
-      <c r="X47" s="127"/>
-      <c r="Y47" s="127"/>
-      <c r="Z47" s="127"/>
-      <c r="AA47" s="127"/>
-      <c r="AB47" s="127"/>
+      <c r="U47" s="70"/>
+      <c r="V47" s="70"/>
+      <c r="W47" s="70"/>
+      <c r="X47" s="70"/>
+      <c r="Y47" s="70"/>
+      <c r="Z47" s="70"/>
+      <c r="AA47" s="70"/>
+      <c r="AB47" s="70"/>
       <c r="AL47" s="12"/>
     </row>
     <row r="48" spans="1:38" ht="14.45" customHeight="1">
@@ -4244,16 +4591,16 @@
       <c r="Q48" s="22"/>
       <c r="R48" s="22"/>
       <c r="S48" s="22"/>
-      <c r="T48" s="139" t="s">
+      <c r="T48" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="U48" s="139"/>
-      <c r="V48" s="139"/>
-      <c r="W48" s="139"/>
-      <c r="X48" s="139"/>
-      <c r="Y48" s="139"/>
-      <c r="Z48" s="139"/>
-      <c r="AA48" s="139"/>
+      <c r="U48" s="43"/>
+      <c r="V48" s="43"/>
+      <c r="W48" s="43"/>
+      <c r="X48" s="43"/>
+      <c r="Y48" s="43"/>
+      <c r="Z48" s="43"/>
+      <c r="AA48" s="43"/>
       <c r="AL48" s="12"/>
     </row>
     <row r="49" spans="1:38" ht="14.45" customHeight="1">
@@ -4299,14 +4646,14 @@
       <c r="Q50" s="26"/>
       <c r="R50" s="26"/>
       <c r="S50" s="26"/>
-      <c r="U50" s="140"/>
-      <c r="V50" s="140"/>
-      <c r="W50" s="140"/>
-      <c r="X50" s="140"/>
-      <c r="Y50" s="140"/>
-      <c r="Z50" s="140"/>
-      <c r="AA50" s="140"/>
-      <c r="AB50" s="140"/>
+      <c r="U50" s="44"/>
+      <c r="V50" s="44"/>
+      <c r="W50" s="44"/>
+      <c r="X50" s="44"/>
+      <c r="Y50" s="44"/>
+      <c r="Z50" s="44"/>
+      <c r="AA50" s="44"/>
+      <c r="AB50" s="44"/>
       <c r="AL50" s="12"/>
     </row>
     <row r="51" spans="1:38">
@@ -4330,16 +4677,16 @@
       <c r="R51" s="12"/>
       <c r="S51" s="12"/>
       <c r="T51" s="14"/>
-      <c r="U51" s="122" t="s">
+      <c r="U51" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="V51" s="123"/>
-      <c r="W51" s="123"/>
-      <c r="X51" s="123"/>
-      <c r="Y51" s="123"/>
-      <c r="Z51" s="123"/>
-      <c r="AA51" s="123"/>
-      <c r="AB51" s="123"/>
+      <c r="V51" s="66"/>
+      <c r="W51" s="66"/>
+      <c r="X51" s="66"/>
+      <c r="Y51" s="66"/>
+      <c r="Z51" s="66"/>
+      <c r="AA51" s="66"/>
+      <c r="AB51" s="66"/>
       <c r="AL51" s="12"/>
     </row>
     <row r="52" spans="1:38">
@@ -4396,19 +4743,102 @@
       <c r="R53" s="12"/>
       <c r="S53" s="12"/>
       <c r="T53" s="12"/>
-      <c r="AC53" s="32"/>
-      <c r="AD53" s="32"/>
-      <c r="AE53" s="32"/>
-      <c r="AF53" s="32"/>
-      <c r="AG53" s="32"/>
-      <c r="AH53" s="32"/>
-      <c r="AI53" s="32"/>
-      <c r="AJ53" s="32"/>
-      <c r="AK53" s="32"/>
+      <c r="AC53" s="31"/>
+      <c r="AD53" s="31"/>
+      <c r="AE53" s="31"/>
+      <c r="AF53" s="31"/>
+      <c r="AG53" s="31"/>
+      <c r="AH53" s="31"/>
+      <c r="AI53" s="31"/>
+      <c r="AJ53" s="31"/>
+      <c r="AK53" s="31"/>
       <c r="AL53" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="99">
+    <mergeCell ref="AD5:AD7"/>
+    <mergeCell ref="R4:X4"/>
+    <mergeCell ref="R3:X3"/>
+    <mergeCell ref="M4:Q4"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="AB4:AD4"/>
+    <mergeCell ref="Y4:AA4"/>
+    <mergeCell ref="A1:AD1"/>
+    <mergeCell ref="A2:AD2"/>
+    <mergeCell ref="C4:L4"/>
+    <mergeCell ref="I3:L3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:AA5"/>
+    <mergeCell ref="AB5:AC6"/>
+    <mergeCell ref="Z23:Z24"/>
+    <mergeCell ref="AA23:AB24"/>
+    <mergeCell ref="T21:V21"/>
+    <mergeCell ref="T22:V22"/>
+    <mergeCell ref="W21:X21"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="K21:R21"/>
+    <mergeCell ref="K22:R23"/>
+    <mergeCell ref="K24:R24"/>
+    <mergeCell ref="Y25:Y28"/>
+    <mergeCell ref="Z25:Z28"/>
+    <mergeCell ref="AA25:AB28"/>
+    <mergeCell ref="T27:X28"/>
+    <mergeCell ref="Y21:AB21"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="T23:X24"/>
+    <mergeCell ref="Y23:Y24"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C28:H28"/>
+    <mergeCell ref="T25:V26"/>
+    <mergeCell ref="W25:X26"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="K25:R25"/>
+    <mergeCell ref="T33:X34"/>
+    <mergeCell ref="T37:X38"/>
+    <mergeCell ref="C26:H26"/>
+    <mergeCell ref="C27:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="K26:R28"/>
+    <mergeCell ref="K29:R29"/>
+    <mergeCell ref="C29:H29"/>
+    <mergeCell ref="C30:H30"/>
+    <mergeCell ref="C31:H31"/>
+    <mergeCell ref="T36:X36"/>
+    <mergeCell ref="AA36:AB36"/>
+    <mergeCell ref="Y29:Y30"/>
+    <mergeCell ref="Z29:Z30"/>
+    <mergeCell ref="AA29:AB30"/>
+    <mergeCell ref="T30:X30"/>
+    <mergeCell ref="T31:X31"/>
+    <mergeCell ref="Y31:Y32"/>
+    <mergeCell ref="T29:X29"/>
+    <mergeCell ref="Z31:Z32"/>
+    <mergeCell ref="AA31:AB32"/>
+    <mergeCell ref="T32:X32"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:D24"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="A34:I36"/>
+    <mergeCell ref="U46:AB47"/>
+    <mergeCell ref="K40:R40"/>
+    <mergeCell ref="T39:X40"/>
+    <mergeCell ref="Y39:Y40"/>
+    <mergeCell ref="Z39:Z40"/>
+    <mergeCell ref="AA39:AB40"/>
+    <mergeCell ref="T41:X42"/>
+    <mergeCell ref="Y41:Y42"/>
+    <mergeCell ref="Y33:Y34"/>
+    <mergeCell ref="Z33:Z34"/>
+    <mergeCell ref="AA33:AB34"/>
+    <mergeCell ref="AA35:AB35"/>
+    <mergeCell ref="K38:R39"/>
+    <mergeCell ref="Y37:Y38"/>
+    <mergeCell ref="Z37:Z38"/>
+    <mergeCell ref="AA37:AB38"/>
+    <mergeCell ref="U51:AB51"/>
     <mergeCell ref="I30:I31"/>
     <mergeCell ref="K30:R33"/>
     <mergeCell ref="K34:R34"/>
@@ -4425,89 +4855,6 @@
     <mergeCell ref="T35:X35"/>
     <mergeCell ref="K35:R36"/>
     <mergeCell ref="K37:R37"/>
-    <mergeCell ref="K38:R39"/>
-    <mergeCell ref="Y37:Y38"/>
-    <mergeCell ref="Z37:Z38"/>
-    <mergeCell ref="AA37:AB38"/>
-    <mergeCell ref="U51:AB51"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:D24"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="A34:I36"/>
-    <mergeCell ref="U46:AB47"/>
-    <mergeCell ref="K40:R40"/>
-    <mergeCell ref="T39:X40"/>
-    <mergeCell ref="Y39:Y40"/>
-    <mergeCell ref="Z39:Z40"/>
-    <mergeCell ref="AA39:AB40"/>
-    <mergeCell ref="T41:X42"/>
-    <mergeCell ref="Y41:Y42"/>
-    <mergeCell ref="Y33:Y34"/>
-    <mergeCell ref="Z33:Z34"/>
-    <mergeCell ref="AA33:AB34"/>
-    <mergeCell ref="AA35:AB35"/>
-    <mergeCell ref="T36:X36"/>
-    <mergeCell ref="AA36:AB36"/>
-    <mergeCell ref="Y29:Y30"/>
-    <mergeCell ref="Z29:Z30"/>
-    <mergeCell ref="AA29:AB30"/>
-    <mergeCell ref="T30:X30"/>
-    <mergeCell ref="T31:X31"/>
-    <mergeCell ref="Y31:Y32"/>
-    <mergeCell ref="T29:X29"/>
-    <mergeCell ref="Z31:Z32"/>
-    <mergeCell ref="AA31:AB32"/>
-    <mergeCell ref="T32:X32"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="C28:H28"/>
-    <mergeCell ref="T25:V26"/>
-    <mergeCell ref="W25:X26"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="K25:R25"/>
-    <mergeCell ref="T33:X34"/>
-    <mergeCell ref="T37:X38"/>
-    <mergeCell ref="C26:H26"/>
-    <mergeCell ref="C27:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="K26:R28"/>
-    <mergeCell ref="K29:R29"/>
-    <mergeCell ref="C29:H29"/>
-    <mergeCell ref="C30:H30"/>
-    <mergeCell ref="C31:H31"/>
-    <mergeCell ref="Y25:Y28"/>
-    <mergeCell ref="Z25:Z28"/>
-    <mergeCell ref="AA25:AB28"/>
-    <mergeCell ref="T27:X28"/>
-    <mergeCell ref="Y21:AB21"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="T23:X24"/>
-    <mergeCell ref="Y23:Y24"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:AA5"/>
-    <mergeCell ref="AB5:AC6"/>
-    <mergeCell ref="Z23:Z24"/>
-    <mergeCell ref="AA23:AB24"/>
-    <mergeCell ref="T21:V21"/>
-    <mergeCell ref="T22:V22"/>
-    <mergeCell ref="W21:X21"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="K21:R21"/>
-    <mergeCell ref="K22:R23"/>
-    <mergeCell ref="K24:R24"/>
-    <mergeCell ref="A1:AD1"/>
-    <mergeCell ref="A2:AD2"/>
-    <mergeCell ref="C4:L4"/>
-    <mergeCell ref="I3:L3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="AD5:AD7"/>
-    <mergeCell ref="R4:X4"/>
-    <mergeCell ref="R3:X3"/>
-    <mergeCell ref="M4:Q4"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="AB4:AD4"/>
-    <mergeCell ref="Y4:AA4"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="65" fitToHeight="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Attendance System Thread
-Fixed adding wrong comma for Failed Subjects... (Shows "CODE ," instead of "CODE, ")
</commit_message>
<xml_diff>
--- a/Project Files/Forms System Final/exports/jh_sf2.xlsx
+++ b/Project Files/Forms System Final/exports/jh_sf2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3760" uniqueCount="114">
   <si>
     <t>M</t>
   </si>
@@ -368,40 +368,43 @@
     <t>1</t>
   </si>
   <si>
+    <t xml:space="preserve">Rizal, Jose </t>
+  </si>
+  <si>
+    <t>T/I: 2020-02-01</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>TLC</t>
+  </si>
+  <si>
+    <t>&lt;==Male Total Per Day==&gt;</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
     <t>Paderogao, Phil Rey, E. Jr</t>
   </si>
   <si>
-    <t>T/I: 2020-02-01</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>TCC</t>
   </si>
   <si>
-    <t xml:space="preserve">Rizal, Jose </t>
-  </si>
-  <si>
-    <t>TLC</t>
-  </si>
-  <si>
-    <t>&lt;==Male Total Per Day==&gt;</t>
-  </si>
-  <si>
     <t>&lt;==Female Total Per Day==&gt;</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
     <t>&lt;==Combined Total Per Day==&gt;</t>
   </si>
   <si>
     <t>100</t>
+  </si>
+  <si>
+    <t>0.5</t>
   </si>
   <si>
     <t>50</t>
@@ -547,11 +550,6 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color rgb="FFFFFF"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <sz val="11.0"/>
       <color rgb="000000"/>
     </font>
     <font>
@@ -567,12 +565,17 @@
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
-      <color rgb="000000"/>
+      <color rgb="FFFFFF"/>
     </font>
     <font>
       <name val="Calibri"/>
       <sz val="11.0"/>
       <color rgb="FFFFFF"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <color rgb="000000"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1875,28 +1878,28 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="70" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="73" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="70" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="73" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="66" xfId="0" applyBorder="true" applyFont="true">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -1999,13 +2002,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>22</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -2037,15 +2040,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2750,31 +2753,31 @@
         <v>103</v>
       </c>
       <c r="N8" s="169" t="s">
+        <v>103</v>
+      </c>
+      <c r="O8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V8" s="170" t="s">
         <v>104</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V8" s="170" t="s">
-        <v>102</v>
       </c>
       <c r="W8" s="1" t="s">
         <v>20</v>
@@ -2803,7 +2806,7 @@
     </row>
     <row r="9" spans="1:30">
       <c r="A9" s="3" t="s">
-        <v>79</v>
+        <v>20</v>
       </c>
       <c r="B9" s="9" t="s">
         <v>105</v>
@@ -2835,14 +2838,14 @@
       <c r="K9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L9" s="171" t="s">
-        <v>103</v>
-      </c>
-      <c r="M9" s="172" t="s">
-        <v>102</v>
-      </c>
-      <c r="N9" s="173" t="s">
-        <v>102</v>
+      <c r="L9" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>99</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>20</v>
@@ -2865,7 +2868,7 @@
       <c r="U9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V9" s="174" t="s">
+      <c r="V9" s="4" t="s">
         <v>106</v>
       </c>
       <c r="W9" s="1" t="s">
@@ -2889,13 +2892,11 @@
       <c r="AC9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="AD9" s="3" t="s">
-        <v>101</v>
-      </c>
+      <c r="AD9" s="3"/>
     </row>
     <row r="10" spans="1:30">
       <c r="A10" s="3" t="s">
-        <v>20</v>
+        <v>79</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>107</v>
@@ -2927,68 +2928,70 @@
       <c r="K10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L10" s="4" t="s">
+      <c r="L10" s="171" t="s">
+        <v>103</v>
+      </c>
+      <c r="M10" s="172" t="s">
+        <v>102</v>
+      </c>
+      <c r="N10" s="173" t="s">
+        <v>108</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="P10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="R10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="T10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V10" s="174" t="s">
+        <v>103</v>
+      </c>
+      <c r="W10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="X10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="AC10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="R10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V10" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="X10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD10" s="3"/>
+      <c r="AD10" s="3" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:30">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>20</v>
@@ -3018,13 +3021,13 @@
         <v>20</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="M11" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="N11" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>20</v>
@@ -3048,7 +3051,7 @@
         <v>20</v>
       </c>
       <c r="V11" s="4" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="W11" s="1" t="s">
         <v>20</v>
@@ -3066,10 +3069,10 @@
         <v>20</v>
       </c>
       <c r="AB11" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AC11" s="3" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AD11" s="3"/>
     </row>
@@ -3881,10 +3884,10 @@
       <c r="W23" s="114"/>
       <c r="X23" s="115"/>
       <c r="Y23" s="119" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="Z23" s="99" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AA23" s="102" t="s">
         <v>79</v>
@@ -3957,13 +3960,13 @@
       </c>
       <c r="X25" s="93"/>
       <c r="Y25" s="99" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z25" s="99" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA25" s="102" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AB25" s="103"/>
       <c r="AL25" s="12"/>
@@ -4109,10 +4112,10 @@
       <c r="W29" s="86"/>
       <c r="X29" s="87"/>
       <c r="Y29" s="53" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="Z29" s="53" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AA29" s="55" t="s">
         <v>79</v>
@@ -4193,7 +4196,7 @@
         <v>111</v>
       </c>
       <c r="Z31" s="53" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="AA31" s="55" t="s">
         <v>111</v>
@@ -4256,13 +4259,13 @@
       <c r="W33" s="96"/>
       <c r="X33" s="97"/>
       <c r="Y33" s="53" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="Z33" s="53" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="AA33" s="55" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="AB33" s="56"/>
       <c r="AL33" s="12"/>
@@ -4332,13 +4335,13 @@
       <c r="W35" s="60"/>
       <c r="X35" s="61"/>
       <c r="Y35" s="33" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="Z35" s="33" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="AA35" s="80" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="AB35" s="81"/>
       <c r="AL35" s="12"/>
@@ -4371,13 +4374,13 @@
       <c r="W36" s="60"/>
       <c r="X36" s="61"/>
       <c r="Y36" s="33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z36" s="33" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA36" s="80" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AB36" s="81"/>
       <c r="AL36" s="12"/>
@@ -4412,13 +4415,13 @@
       <c r="W37" s="72"/>
       <c r="X37" s="73"/>
       <c r="Y37" s="53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z37" s="53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA37" s="55" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AB37" s="56"/>
       <c r="AL37" s="12"/>
@@ -4486,13 +4489,13 @@
       <c r="W39" s="72"/>
       <c r="X39" s="73"/>
       <c r="Y39" s="53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="Z39" s="53" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AA39" s="55" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="AB39" s="56"/>
       <c r="AL39" s="12"/>
@@ -4560,10 +4563,10 @@
       <c r="W41" s="72"/>
       <c r="X41" s="73"/>
       <c r="Y41" s="53" t="s">
-        <v>79</v>
+        <v>99</v>
       </c>
       <c r="Z41" s="53" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="AA41" s="55" t="s">
         <v>79</v>

</xml_diff>